<commit_message>
Registro de pruebas - correcciones
</commit_message>
<xml_diff>
--- a/Registro de Pruebas T1 INF331.xlsx
+++ b/Registro de Pruebas T1 INF331.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DIEGO VEAS BASTIAS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F92E02-4E71-4FAC-927B-C41404E42F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE799EC-5011-4833-817D-04D17864C167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -579,8 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -972,8 +970,8 @@
   </sheetPr>
   <dimension ref="A2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -987,10 +985,10 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
@@ -998,35 +996,27 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G6" s="4"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>0</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
@@ -1034,9 +1024,9 @@
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
     </row>
-    <row r="13" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>6</v>
+    <row r="13" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>1</v>
@@ -1055,8 +1045,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
-        <v>1</v>
+      <c r="A14" s="21" t="s">
+        <v>6</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>7</v>
@@ -1075,8 +1065,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>2</v>
+      <c r="A15" s="17">
+        <v>1</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>12</v>
@@ -1094,7 +1084,7 @@
     </row>
     <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>16</v>
@@ -1114,7 +1104,7 @@
     </row>
     <row r="17" spans="1:6" ht="120" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>20</v>
@@ -1134,7 +1124,7 @@
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>24</v>
@@ -1154,7 +1144,7 @@
     </row>
     <row r="19" spans="1:6" ht="120" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>28</v>
@@ -1174,7 +1164,7 @@
     </row>
     <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>32</v>
@@ -1192,7 +1182,7 @@
     </row>
     <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>35</v>
@@ -1212,7 +1202,7 @@
     </row>
     <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>39</v>
@@ -1232,7 +1222,7 @@
     </row>
     <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>44</v>
@@ -1252,7 +1242,7 @@
     </row>
     <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>48</v>
@@ -1270,7 +1260,7 @@
     </row>
     <row r="25" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>51</v>
@@ -1290,7 +1280,7 @@
     </row>
     <row r="26" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>55</v>
@@ -1308,9 +1298,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>59</v>
@@ -1328,7 +1318,7 @@
     </row>
     <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>62</v>
@@ -1345,7 +1335,9 @@
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="6">
+        <v>15</v>
+      </c>
       <c r="B29" s="7" t="s">
         <v>65</v>
       </c>
@@ -1362,24 +1354,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+    </row>
+    <row r="32" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
         <v>6</v>
-      </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-    </row>
-    <row r="32" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17">
-        <v>1</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>7</v>
@@ -1398,8 +1388,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
-        <v>2</v>
+      <c r="A33" s="17">
+        <v>1</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>12</v>
@@ -1417,7 +1407,7 @@
     </row>
     <row r="34" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>16</v>
@@ -1437,7 +1427,7 @@
     </row>
     <row r="35" spans="1:6" ht="135" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>20</v>
@@ -1457,7 +1447,7 @@
     </row>
     <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>24</v>
@@ -1477,7 +1467,7 @@
     </row>
     <row r="37" spans="1:6" ht="120" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>28</v>
@@ -1497,7 +1487,7 @@
     </row>
     <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>32</v>
@@ -1517,7 +1507,7 @@
     </row>
     <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>39</v>
@@ -1537,7 +1527,7 @@
     </row>
     <row r="40" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>35</v>
@@ -1557,7 +1547,7 @@
     </row>
     <row r="41" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>44</v>
@@ -1577,7 +1567,7 @@
     </row>
     <row r="42" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>48</v>
@@ -1593,9 +1583,9 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>51</v>
@@ -1615,7 +1605,7 @@
     </row>
     <row r="44" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>55</v>
@@ -1635,7 +1625,7 @@
     </row>
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>59</v>
@@ -1653,7 +1643,7 @@
     </row>
     <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>62</v>
@@ -1670,6 +1660,9 @@
       <c r="F46" s="12"/>
     </row>
     <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>15</v>
+      </c>
       <c r="B47" s="12" t="s">
         <v>65</v>
       </c>
@@ -1686,24 +1679,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30" t="s">
+    <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="21" t="s">
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+    </row>
+    <row r="50" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="21" t="s">
         <v>6</v>
-      </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-    </row>
-    <row r="50" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="17">
-        <v>1</v>
       </c>
       <c r="B50" s="21" t="s">
         <v>7</v>
@@ -1722,6 +1711,9 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="A51" s="17">
+        <v>1</v>
+      </c>
       <c r="B51" s="18" t="s">
         <v>35</v>
       </c>

</xml_diff>